<commit_message>
Identified JADE-CCM 5.2.2 mapping elements in mapping spreadsheet
</commit_message>
<xml_diff>
--- a/mapping/docs/DEMS Integration Data Mapping v1.13 Daniel Conti Aug 2 - mapping status.xlsx
+++ b/mapping/docs/DEMS Integration Data Mapping v1.13 Daniel Conti Aug 2 - mapping status.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\justice\dems\jpss-jade-ccm\mapping\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git\jade\jpss-jade-ccm\mapping\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE20B9FD-8D14-45D4-85F8-66CF3CB60892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAB6349-F516-48F9-B671-5BF783EBB58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28710" yWindow="750" windowWidth="19620" windowHeight="19485" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0. Change Log" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1961" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2003" uniqueCount="647">
   <si>
     <t>Change Date</t>
   </si>
@@ -3390,6 +3390,12 @@
   </si>
   <si>
     <t>CRN_DECISION_AGENCY_NAME</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>JADE-CCM 5.2.2</t>
   </si>
 </sst>
 </file>
@@ -5617,9 +5623,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A292DBCF-B35F-4E38-91EC-93A3024A386F}" name="Table2" displayName="Table2" ref="A1:X92" totalsRowShown="0" headerRowDxfId="28" dataDxfId="26" headerRowBorderDxfId="27" tableBorderDxfId="25" totalsRowBorderDxfId="24" headerRowCellStyle="Good">
   <autoFilter ref="A1:X92" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="5">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
+      <filters>
+        <filter val="JADE-CCM 5.2.2"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="24">
@@ -6498,10 +6504,10 @@
   <dimension ref="A1:AB92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6609,7 +6615,7 @@
       <c r="Z1" s="77"/>
       <c r="AB1" s="77"/>
     </row>
-    <row r="2" spans="1:28" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="65">
         <v>1</v>
       </c>
@@ -6629,7 +6635,7 @@
         <v>641</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>109</v>
@@ -6679,7 +6685,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="2" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" s="2" customFormat="1" ht="255" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="65">
         <v>2</v>
       </c>
@@ -6699,7 +6705,7 @@
         <v>641</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>122</v>
@@ -6841,7 +6847,7 @@
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
     </row>
-    <row r="6" spans="1:28" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" s="2" customFormat="1" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="65">
         <v>5</v>
       </c>
@@ -6861,7 +6867,7 @@
         <v>641</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>138</v>
@@ -6915,7 +6921,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="7" spans="1:28" s="2" customFormat="1" ht="240" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" s="2" customFormat="1" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="65">
         <v>6</v>
       </c>
@@ -6935,7 +6941,7 @@
         <v>641</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>106</v>
@@ -6989,7 +6995,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:28" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" s="2" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="65">
         <v>7</v>
       </c>
@@ -7009,7 +7015,7 @@
         <v>641</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>152</v>
@@ -7061,7 +7067,7 @@
       </c>
       <c r="X8" s="7"/>
     </row>
-    <row r="9" spans="1:28" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="65">
         <v>8</v>
       </c>
@@ -7081,7 +7087,7 @@
         <v>641</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>157</v>
@@ -7136,7 +7142,7 @@
       <c r="Z9" s="77"/>
       <c r="AB9" s="77"/>
     </row>
-    <row r="10" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="65">
         <v>9</v>
       </c>
@@ -7156,7 +7162,7 @@
         <v>641</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>164</v>
@@ -7211,7 +7217,7 @@
       <c r="Z10" s="77"/>
       <c r="AB10" s="77"/>
     </row>
-    <row r="11" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="65">
         <v>10</v>
       </c>
@@ -7231,7 +7237,7 @@
         <v>641</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>170</v>
@@ -7286,7 +7292,7 @@
       <c r="Z11" s="77"/>
       <c r="AB11" s="77"/>
     </row>
-    <row r="12" spans="1:28" ht="90" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="65">
         <v>11</v>
       </c>
@@ -7306,7 +7312,7 @@
         <v>641</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>176</v>
@@ -7361,7 +7367,7 @@
       <c r="Z12" s="77"/>
       <c r="AB12" s="77"/>
     </row>
-    <row r="13" spans="1:28" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="65">
         <v>12</v>
       </c>
@@ -7381,7 +7387,7 @@
         <v>641</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>185</v>
@@ -7436,7 +7442,7 @@
       <c r="Z13" s="77"/>
       <c r="AB13" s="77"/>
     </row>
-    <row r="14" spans="1:28" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" s="2" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="65">
         <v>13</v>
       </c>
@@ -7456,7 +7462,7 @@
         <v>641</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>192</v>
@@ -7508,7 +7514,7 @@
       </c>
       <c r="X14" s="7"/>
     </row>
-    <row r="15" spans="1:28" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="65">
         <v>14</v>
       </c>
@@ -7528,7 +7534,7 @@
         <v>641</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>196</v>
@@ -7576,7 +7582,7 @@
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
     </row>
-    <row r="16" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="65">
         <v>15</v>
       </c>
@@ -7596,7 +7602,7 @@
         <v>641</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>198</v>
@@ -7647,7 +7653,7 @@
       <c r="Z16" s="77"/>
       <c r="AB16" s="77"/>
     </row>
-    <row r="17" spans="1:24" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" s="2" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="65">
         <v>16</v>
       </c>
@@ -7667,7 +7673,7 @@
         <v>641</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>204</v>
@@ -7719,7 +7725,7 @@
       </c>
       <c r="X17" s="7"/>
     </row>
-    <row r="18" spans="1:24" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" s="2" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="65">
         <v>17</v>
       </c>
@@ -7739,7 +7745,7 @@
         <v>641</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>106</v>
@@ -7791,7 +7797,7 @@
       </c>
       <c r="X18" s="66"/>
     </row>
-    <row r="19" spans="1:24" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" s="2" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="65">
         <v>18</v>
       </c>
@@ -7811,7 +7817,7 @@
         <v>641</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>215</v>
@@ -7863,7 +7869,7 @@
       </c>
       <c r="X19" s="7"/>
     </row>
-    <row r="20" spans="1:24" s="2" customFormat="1" ht="300" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" s="2" customFormat="1" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="65">
         <v>19</v>
       </c>
@@ -7883,7 +7889,7 @@
         <v>641</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H20" s="7" t="s">
         <v>224</v>
@@ -7937,7 +7943,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="21" spans="1:24" s="2" customFormat="1" ht="285" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" s="2" customFormat="1" ht="285" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="65">
         <v>20</v>
       </c>
@@ -7957,7 +7963,7 @@
         <v>641</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H21" s="7" t="s">
         <v>232</v>
@@ -8011,7 +8017,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="22" spans="1:24" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" s="2" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="65">
         <v>21</v>
       </c>
@@ -8031,7 +8037,7 @@
         <v>641</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H22" s="7" t="s">
         <v>243</v>
@@ -8081,7 +8087,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="23" spans="1:24" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" s="2" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="65">
         <v>22</v>
       </c>
@@ -8101,7 +8107,7 @@
         <v>641</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H23" s="7" t="s">
         <v>252</v>
@@ -8155,7 +8161,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="24" spans="1:24" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" s="2" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="65">
         <v>23</v>
       </c>
@@ -8175,7 +8181,7 @@
         <v>641</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>261</v>
@@ -8229,7 +8235,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="25" spans="1:24" s="2" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" s="2" customFormat="1" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="65">
         <v>24</v>
       </c>
@@ -8249,7 +8255,7 @@
         <v>641</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H25" s="7" t="s">
         <v>270</v>
@@ -8303,7 +8309,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="26" spans="1:24" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" s="2" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="65">
         <v>25</v>
       </c>
@@ -8323,7 +8329,7 @@
         <v>641</v>
       </c>
       <c r="G26" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H26" s="7" t="s">
         <v>277</v>
@@ -8377,7 +8383,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="27" spans="1:24" s="2" customFormat="1" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" s="2" customFormat="1" ht="409.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="65">
         <v>26</v>
       </c>
@@ -8397,7 +8403,7 @@
         <v>641</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H27" s="7" t="s">
         <v>283</v>
@@ -8447,7 +8453,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="28" spans="1:24" s="2" customFormat="1" ht="330" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" s="2" customFormat="1" ht="330" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="65">
         <v>27</v>
       </c>
@@ -8467,7 +8473,7 @@
         <v>641</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H28" s="7" t="s">
         <v>289</v>
@@ -8521,7 +8527,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="29" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="65">
         <v>28</v>
       </c>
@@ -8537,7 +8543,9 @@
       <c r="E29" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F29" s="7"/>
+      <c r="F29" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7" t="s">
         <v>298</v>
@@ -8585,7 +8593,7 @@
       <c r="W29" s="7"/>
       <c r="X29" s="12"/>
     </row>
-    <row r="30" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="65">
         <v>29</v>
       </c>
@@ -8601,7 +8609,9 @@
       <c r="E30" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="F30" s="7"/>
+      <c r="F30" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G30" s="7"/>
       <c r="H30" s="7" t="s">
         <v>307</v>
@@ -8653,7 +8663,7 @@
       </c>
       <c r="X30" s="9"/>
     </row>
-    <row r="31" spans="1:24" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A31" s="65">
         <v>30</v>
       </c>
@@ -8669,7 +8679,9 @@
       <c r="E31" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="F31" s="7"/>
+      <c r="F31" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G31" s="7"/>
       <c r="H31" s="7" t="s">
         <v>313</v>
@@ -8723,7 +8735,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="32" spans="1:24" s="2" customFormat="1" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" s="2" customFormat="1" ht="195" x14ac:dyDescent="0.25">
       <c r="A32" s="65">
         <v>31</v>
       </c>
@@ -8739,7 +8751,9 @@
       <c r="E32" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F32" s="7"/>
+      <c r="F32" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7" t="s">
         <v>321</v>
@@ -8789,7 +8803,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="33" spans="1:25" s="9" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" s="9" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A33" s="65">
         <v>32</v>
       </c>
@@ -8805,7 +8819,9 @@
       <c r="E33" s="78" t="s">
         <v>300</v>
       </c>
-      <c r="F33" s="78"/>
+      <c r="F33" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G33" s="78"/>
       <c r="H33" s="78" t="s">
         <v>325</v>
@@ -8860,7 +8876,7 @@
       </c>
       <c r="Y33" s="15"/>
     </row>
-    <row r="34" spans="1:25" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="65">
         <v>33</v>
       </c>
@@ -8876,7 +8892,9 @@
       <c r="E34" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="F34" s="7"/>
+      <c r="F34" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G34" s="7"/>
       <c r="H34" s="7" t="s">
         <v>336</v>
@@ -8930,7 +8948,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="35" spans="1:25" s="2" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A35" s="65">
         <v>34</v>
       </c>
@@ -8946,7 +8964,9 @@
       <c r="E35" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="F35" s="7"/>
+      <c r="F35" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G35" s="7"/>
       <c r="H35" s="7" t="s">
         <v>345</v>
@@ -9000,7 +9020,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="36" spans="1:25" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="65">
         <v>35</v>
       </c>
@@ -9016,7 +9036,9 @@
       <c r="E36" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="F36" s="7"/>
+      <c r="F36" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G36" s="7"/>
       <c r="H36" s="7" t="s">
         <v>354</v>
@@ -9068,7 +9090,7 @@
       </c>
       <c r="X36" s="7"/>
     </row>
-    <row r="37" spans="1:25" s="2" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A37" s="65">
         <v>36</v>
       </c>
@@ -9084,7 +9106,9 @@
       <c r="E37" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="F37" s="13"/>
+      <c r="F37" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G37" s="13"/>
       <c r="H37" s="7" t="s">
         <v>363</v>
@@ -9136,7 +9160,7 @@
       </c>
       <c r="X37" s="7"/>
     </row>
-    <row r="38" spans="1:25" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="65">
         <v>37</v>
       </c>
@@ -9152,7 +9176,9 @@
       <c r="E38" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="F38" s="7"/>
+      <c r="F38" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G38" s="7"/>
       <c r="H38" s="7" t="s">
         <v>371</v>
@@ -9342,7 +9368,7 @@
       </c>
       <c r="X40" s="7"/>
     </row>
-    <row r="41" spans="1:25" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
       <c r="A41" s="65">
         <v>40</v>
       </c>
@@ -9358,7 +9384,9 @@
       <c r="E41" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F41" s="78"/>
+      <c r="F41" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G41" s="78"/>
       <c r="H41" s="78" t="s">
         <v>397</v>
@@ -9408,7 +9436,7 @@
       <c r="W41" s="20"/>
       <c r="X41" s="7"/>
     </row>
-    <row r="42" spans="1:25" s="2" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A42" s="65">
         <v>41</v>
       </c>
@@ -9424,7 +9452,9 @@
       <c r="E42" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F42" s="7"/>
+      <c r="F42" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G42" s="7"/>
       <c r="H42" s="7" t="s">
         <v>401</v>
@@ -9476,7 +9506,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="43" spans="1:25" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A43" s="65">
         <v>42</v>
       </c>
@@ -9492,7 +9522,9 @@
       <c r="E43" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F43" s="7"/>
+      <c r="F43" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G43" s="7"/>
       <c r="H43" s="7" t="s">
         <v>405</v>
@@ -9544,7 +9576,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" s="65">
         <v>43</v>
       </c>
@@ -9560,7 +9592,9 @@
       <c r="E44" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F44" s="7"/>
+      <c r="F44" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G44" s="7"/>
       <c r="H44" s="7" t="s">
         <v>411</v>
@@ -9612,7 +9646,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="2" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A45" s="65">
         <v>44</v>
       </c>
@@ -9628,7 +9662,9 @@
       <c r="E45" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F45" s="7"/>
+      <c r="F45" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G45" s="7"/>
       <c r="H45" s="7" t="s">
         <v>415</v>
@@ -9682,7 +9718,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="46" spans="1:25" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
       <c r="A46" s="65">
         <v>45</v>
       </c>
@@ -9698,7 +9734,9 @@
       <c r="E46" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F46" s="78"/>
+      <c r="F46" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G46" s="78"/>
       <c r="H46" s="78" t="s">
         <v>419</v>
@@ -9748,7 +9786,7 @@
       </c>
       <c r="X46" s="75"/>
     </row>
-    <row r="47" spans="1:25" s="2" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" s="2" customFormat="1" ht="142.5" x14ac:dyDescent="0.25">
       <c r="A47" s="65">
         <v>46</v>
       </c>
@@ -9764,7 +9802,9 @@
       <c r="E47" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F47" s="7"/>
+      <c r="F47" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G47" s="7"/>
       <c r="H47" s="78" t="s">
         <v>423</v>
@@ -9816,7 +9856,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="48" spans="1:25" s="2" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A48" s="65">
         <v>47</v>
       </c>
@@ -9832,7 +9872,9 @@
       <c r="E48" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F48" s="7"/>
+      <c r="F48" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G48" s="7"/>
       <c r="H48" s="78" t="s">
         <v>428</v>
@@ -9884,7 +9926,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="49" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="65">
         <v>48</v>
       </c>
@@ -9900,7 +9942,9 @@
       <c r="E49" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F49" s="7"/>
+      <c r="F49" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G49" s="7"/>
       <c r="H49" s="7" t="s">
         <v>435</v>
@@ -9948,7 +9992,7 @@
       </c>
       <c r="X49" s="7"/>
     </row>
-    <row r="50" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="65">
         <v>49</v>
       </c>
@@ -9964,7 +10008,9 @@
       <c r="E50" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="F50" s="78"/>
+      <c r="F50" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G50" s="78"/>
       <c r="H50" s="78" t="s">
         <v>440</v>
@@ -10012,7 +10058,7 @@
       </c>
       <c r="X50" s="78"/>
     </row>
-    <row r="51" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="65">
         <v>50</v>
       </c>
@@ -10028,7 +10074,9 @@
       <c r="E51" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="F51" s="7"/>
+      <c r="F51" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G51" s="7"/>
       <c r="H51" s="7" t="s">
         <v>443</v>
@@ -10076,7 +10124,7 @@
       </c>
       <c r="X51" s="12"/>
     </row>
-    <row r="52" spans="1:24" s="2" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A52" s="65">
         <v>51</v>
       </c>
@@ -10092,7 +10140,9 @@
       <c r="E52" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F52" s="7"/>
+      <c r="F52" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G52" s="7"/>
       <c r="H52" s="7" t="s">
         <v>448</v>
@@ -10142,7 +10192,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="53" spans="1:24" s="2" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" s="65">
         <v>52</v>
       </c>
@@ -10158,7 +10208,9 @@
       <c r="E53" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F53" s="7"/>
+      <c r="F53" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G53" s="7"/>
       <c r="H53" s="7" t="s">
         <v>453</v>
@@ -10208,7 +10260,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="54" spans="1:24" s="2" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.25">
       <c r="A54" s="65">
         <v>53</v>
       </c>
@@ -10224,7 +10276,9 @@
       <c r="E54" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F54" s="7"/>
+      <c r="F54" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G54" s="7"/>
       <c r="H54" s="7" t="s">
         <v>458</v>
@@ -10278,7 +10332,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="55" spans="1:24" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A55" s="65">
         <v>54</v>
       </c>
@@ -10294,7 +10348,9 @@
       <c r="E55" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F55" s="7"/>
+      <c r="F55" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G55" s="7"/>
       <c r="H55" s="7" t="s">
         <v>464</v>
@@ -10348,7 +10404,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:24" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A56" s="65">
         <v>55</v>
       </c>
@@ -10364,7 +10420,9 @@
       <c r="E56" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F56" s="7"/>
+      <c r="F56" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G56" s="7"/>
       <c r="H56" s="7" t="s">
         <v>469</v>
@@ -10418,7 +10476,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="57" spans="1:24" s="2" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.25">
       <c r="A57" s="65">
         <v>56</v>
       </c>
@@ -10434,7 +10492,9 @@
       <c r="E57" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F57" s="7"/>
+      <c r="F57" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G57" s="7"/>
       <c r="H57" s="7" t="s">
         <v>473</v>
@@ -10488,7 +10548,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="58" spans="1:24" s="2" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A58" s="65">
         <v>57</v>
       </c>
@@ -10504,7 +10564,9 @@
       <c r="E58" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F58" s="7"/>
+      <c r="F58" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G58" s="7"/>
       <c r="H58" s="7" t="s">
         <v>478</v>
@@ -10556,7 +10618,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="59" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="65">
         <v>58</v>
       </c>
@@ -10572,7 +10634,9 @@
       <c r="E59" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="F59" s="7"/>
+      <c r="F59" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G59" s="7"/>
       <c r="H59" s="7" t="s">
         <v>484</v>
@@ -10622,7 +10686,7 @@
       </c>
       <c r="X59" s="7"/>
     </row>
-    <row r="60" spans="1:24" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="65">
         <v>59</v>
       </c>
@@ -10642,7 +10706,7 @@
         <v>641</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>488</v>
@@ -10692,7 +10756,7 @@
       </c>
       <c r="X60" s="7"/>
     </row>
-    <row r="61" spans="1:24" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="65">
         <v>60</v>
       </c>
@@ -10712,7 +10776,7 @@
         <v>641</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H61" s="7" t="s">
         <v>161</v>
@@ -10762,7 +10826,7 @@
       </c>
       <c r="X61" s="7"/>
     </row>
-    <row r="62" spans="1:24" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="65">
         <v>61</v>
       </c>
@@ -10782,7 +10846,7 @@
         <v>641</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H62" s="7" t="s">
         <v>493</v>
@@ -10830,7 +10894,7 @@
       <c r="W62" s="9"/>
       <c r="X62" s="7"/>
     </row>
-    <row r="63" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="65">
         <v>62</v>
       </c>
@@ -10846,7 +10910,9 @@
       <c r="E63" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="F63" s="92"/>
+      <c r="F63" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G63" s="92"/>
       <c r="H63" s="7" t="s">
         <v>499</v>
@@ -10898,7 +10964,7 @@
       </c>
       <c r="X63" s="7"/>
     </row>
-    <row r="64" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="65">
         <v>63</v>
       </c>
@@ -10914,7 +10980,9 @@
       <c r="E64" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="F64" s="7"/>
+      <c r="F64" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G64" s="7"/>
       <c r="H64" s="7" t="s">
         <v>502</v>
@@ -10964,7 +11032,7 @@
       </c>
       <c r="X64" s="7"/>
     </row>
-    <row r="65" spans="1:28" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:28" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="65">
         <v>64</v>
       </c>
@@ -10984,7 +11052,7 @@
         <v>642</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H65" s="7" t="s">
         <v>109</v>
@@ -11032,7 +11100,7 @@
       <c r="W65" s="9"/>
       <c r="X65" s="7"/>
     </row>
-    <row r="66" spans="1:28" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" s="2" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="65">
         <v>65</v>
       </c>
@@ -11052,7 +11120,7 @@
         <v>642</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H66" s="7" t="s">
         <v>511</v>
@@ -11100,7 +11168,7 @@
       <c r="W66" s="9"/>
       <c r="X66" s="7"/>
     </row>
-    <row r="67" spans="1:28" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="65">
         <v>66</v>
       </c>
@@ -11120,7 +11188,7 @@
         <v>642</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H67" s="7" t="s">
         <v>518</v>
@@ -11168,7 +11236,7 @@
       <c r="W67" s="9"/>
       <c r="X67" s="7"/>
     </row>
-    <row r="68" spans="1:28" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" s="2" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="65">
         <v>67</v>
       </c>
@@ -11188,7 +11256,7 @@
         <v>642</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H68" s="7" t="s">
         <v>524</v>
@@ -11236,7 +11304,7 @@
       <c r="W68" s="9"/>
       <c r="X68" s="7"/>
     </row>
-    <row r="69" spans="1:28" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:28" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="65">
         <v>68</v>
       </c>
@@ -11256,7 +11324,7 @@
         <v>642</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H69" s="7" t="s">
         <v>531</v>
@@ -11304,7 +11372,7 @@
       <c r="W69" s="9"/>
       <c r="X69" s="7"/>
     </row>
-    <row r="70" spans="1:28" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:28" s="2" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="65">
         <v>69</v>
       </c>
@@ -11324,7 +11392,7 @@
         <v>641</v>
       </c>
       <c r="G70" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H70" s="78" t="s">
         <v>536</v>
@@ -11374,7 +11442,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:28" s="2" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="70">
         <v>70</v>
       </c>
@@ -11394,7 +11462,7 @@
         <v>641</v>
       </c>
       <c r="G71" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H71" s="72" t="s">
         <v>542</v>
@@ -11442,7 +11510,7 @@
       <c r="W71" s="73"/>
       <c r="X71" s="72"/>
     </row>
-    <row r="72" spans="1:28" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:28" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="65">
         <v>71</v>
       </c>
@@ -11462,7 +11530,7 @@
         <v>641</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H72" s="91" t="s">
         <v>544</v>
@@ -11514,7 +11582,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="2" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:28" s="2" customFormat="1" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="65">
         <v>72</v>
       </c>
@@ -11534,7 +11602,7 @@
         <v>641</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H73" s="72" t="s">
         <v>549</v>
@@ -11582,7 +11650,7 @@
       <c r="W73" s="73"/>
       <c r="X73" s="72"/>
     </row>
-    <row r="74" spans="1:28" ht="90" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:28" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="70">
         <v>73</v>
       </c>
@@ -11602,7 +11670,7 @@
         <v>641</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H74" s="91" t="s">
         <v>553</v>
@@ -11653,7 +11721,7 @@
       <c r="Z74" s="77"/>
       <c r="AB74" s="77"/>
     </row>
-    <row r="75" spans="1:28" ht="135" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:28" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="65">
         <v>74</v>
       </c>
@@ -11673,7 +11741,7 @@
         <v>641</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H75" s="7" t="s">
         <v>555</v>
@@ -11728,7 +11796,7 @@
       <c r="Z75" s="77"/>
       <c r="AB75" s="77"/>
     </row>
-    <row r="76" spans="1:28" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="70">
         <v>75</v>
       </c>
@@ -11744,7 +11812,9 @@
       <c r="E76" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="F76" s="91"/>
+      <c r="F76" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G76" s="91"/>
       <c r="H76" s="91" t="s">
         <v>559</v>
@@ -11797,7 +11867,7 @@
       <c r="Z76" s="77"/>
       <c r="AB76" s="77"/>
     </row>
-    <row r="77" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="70">
         <v>76</v>
       </c>
@@ -11813,7 +11883,9 @@
       <c r="E77" s="91" t="s">
         <v>627</v>
       </c>
-      <c r="F77" s="91"/>
+      <c r="F77" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G77" s="91"/>
       <c r="H77" s="91" t="s">
         <v>564</v>
@@ -11864,7 +11936,7 @@
       <c r="Z77" s="77"/>
       <c r="AB77" s="77"/>
     </row>
-    <row r="78" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="70">
         <v>77</v>
       </c>
@@ -11880,7 +11952,9 @@
       <c r="E78" s="91" t="s">
         <v>627</v>
       </c>
-      <c r="F78" s="91"/>
+      <c r="F78" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G78" s="91"/>
       <c r="H78" s="91" t="s">
         <v>567</v>
@@ -11931,7 +12005,7 @@
       <c r="Z78" s="77"/>
       <c r="AB78" s="77"/>
     </row>
-    <row r="79" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="65">
         <v>78</v>
       </c>
@@ -11951,7 +12025,7 @@
         <v>641</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H79" s="7" t="s">
         <v>574</v>
@@ -12000,7 +12074,7 @@
       <c r="Z79" s="77"/>
       <c r="AB79" s="77"/>
     </row>
-    <row r="80" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="70">
         <v>79</v>
       </c>
@@ -12016,7 +12090,9 @@
       <c r="E80" s="78" t="s">
         <v>142</v>
       </c>
-      <c r="F80" s="78"/>
+      <c r="F80" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G80" s="78"/>
       <c r="H80" s="7" t="s">
         <v>574</v>
@@ -12065,7 +12141,7 @@
       <c r="Z80" s="77"/>
       <c r="AB80" s="77"/>
     </row>
-    <row r="81" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="70">
         <v>80</v>
       </c>
@@ -12081,7 +12157,9 @@
       <c r="E81" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="F81" s="7"/>
+      <c r="F81" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G81" s="7"/>
       <c r="H81" s="7" t="s">
         <v>192</v>
@@ -12132,7 +12210,7 @@
       <c r="Z81" s="77"/>
       <c r="AB81" s="77"/>
     </row>
-    <row r="82" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="65">
         <v>81</v>
       </c>
@@ -12148,7 +12226,9 @@
       <c r="E82" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="F82" s="7"/>
+      <c r="F82" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G82" s="7"/>
       <c r="H82" s="7" t="s">
         <v>185</v>
@@ -12199,7 +12279,7 @@
       <c r="Z82" s="77"/>
       <c r="AB82" s="77"/>
     </row>
-    <row r="83" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="70">
         <v>82</v>
       </c>
@@ -12215,7 +12295,9 @@
       <c r="E83" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="F83" s="78"/>
+      <c r="F83" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G83" s="78"/>
       <c r="H83" s="7" t="s">
         <v>555</v>
@@ -12266,7 +12348,7 @@
       <c r="Z83" s="77"/>
       <c r="AB83" s="77"/>
     </row>
-    <row r="84" spans="1:28" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" ht="60" x14ac:dyDescent="0.25">
       <c r="A84" s="70">
         <v>83</v>
       </c>
@@ -12282,7 +12364,9 @@
       <c r="E84" s="91" t="s">
         <v>142</v>
       </c>
-      <c r="F84" s="91"/>
+      <c r="F84" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G84" s="91"/>
       <c r="H84" s="91" t="s">
         <v>536</v>
@@ -12333,7 +12417,7 @@
       <c r="Z84" s="77"/>
       <c r="AB84" s="77"/>
     </row>
-    <row r="85" spans="1:28" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A85" s="70">
         <v>84</v>
       </c>
@@ -12349,7 +12433,9 @@
       <c r="E85" s="78" t="s">
         <v>142</v>
       </c>
-      <c r="F85" s="96"/>
+      <c r="F85" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G85" s="96"/>
       <c r="H85" s="78" t="s">
         <v>578</v>
@@ -12378,7 +12464,7 @@
       <c r="Z85" s="77"/>
       <c r="AB85" s="77"/>
     </row>
-    <row r="86" spans="1:28" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A86" s="65">
         <v>85</v>
       </c>
@@ -12394,7 +12480,9 @@
       <c r="E86" s="78" t="s">
         <v>142</v>
       </c>
-      <c r="F86" s="97"/>
+      <c r="F86" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G86" s="97"/>
       <c r="H86" s="91" t="s">
         <v>579</v>
@@ -12421,7 +12509,7 @@
       <c r="Z86" s="77"/>
       <c r="AB86" s="77"/>
     </row>
-    <row r="87" spans="1:28" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" ht="75" x14ac:dyDescent="0.25">
       <c r="A87" s="70">
         <v>86</v>
       </c>
@@ -12437,7 +12525,9 @@
       <c r="E87" s="78" t="s">
         <v>142</v>
       </c>
-      <c r="F87" s="97"/>
+      <c r="F87" s="7" t="s">
+        <v>646</v>
+      </c>
       <c r="G87" s="97"/>
       <c r="H87" s="91" t="s">
         <v>580</v>
@@ -12464,7 +12554,7 @@
       <c r="Z87" s="77"/>
       <c r="AB87" s="77"/>
     </row>
-    <row r="88" spans="1:28" ht="90" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:28" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="70">
         <v>87</v>
       </c>
@@ -12484,7 +12574,7 @@
         <v>641</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>218</v>
+        <v>645</v>
       </c>
       <c r="H88" s="91" t="s">
         <v>630</v>
@@ -13980,6 +14070,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004309D8389C5A084A8EB9FED342634609" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c1ee2663b349001e41875756695405cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e8508775-6f2a-451e-b0c0-0da0ba3b654b" xmlns:ns3="f15e5eab-f649-4efd-a2c2-4935b72130ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6561bc30f91fc8f80cc55469271a584" ns2:_="" ns3:_="">
     <xsd:import namespace="e8508775-6f2a-451e-b0c0-0da0ba3b654b"/>
@@ -14144,12 +14240,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -14160,6 +14250,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6ECE83-F240-478D-BE60-3B98A1630AA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA6218BD-C386-4EBA-AE3F-6A1B03CAFB13}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14178,15 +14277,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6ECE83-F240-478D-BE60-3B98A1630AA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91500E67-CFBD-4E57-93CA-25297AD67667}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
data model names refactoring and documentation
</commit_message>
<xml_diff>
--- a/mapping/docs/DEMS Integration Data Mapping v1.13 Daniel Conti Aug 2 - mapping status.xlsx
+++ b/mapping/docs/DEMS Integration Data Mapping v1.13 Daniel Conti Aug 2 - mapping status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\git\jade\jpss-jade-ccm\mapping\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAB6349-F516-48F9-B671-5BF783EBB58E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ED7361-25AD-4DC3-B99A-5B808FCF3D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0. Change Log" sheetId="3" r:id="rId1"/>
@@ -5627,6 +5627,20 @@
         <filter val="JADE-CCM 5.2.2"/>
       </filters>
     </filterColumn>
+    <filterColumn colId="9">
+      <filters>
+        <filter val="getCourtFile"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="19">
+      <filters>
+        <filter val="Class"/>
+        <filter val="Court File Level"/>
+        <filter val="Crown Election"/>
+        <filter val="Designation"/>
+        <filter val="Sworn Date"/>
+      </filters>
+    </filterColumn>
   </autoFilter>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{835DEB9C-EF50-49F3-AADC-8EEC259AD441}" name="#" dataDxfId="23"/>
@@ -6504,10 +6518,10 @@
   <dimension ref="A1:AB92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomRight" activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8527,7 +8541,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="29" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="65">
         <v>28</v>
       </c>
@@ -8593,7 +8607,7 @@
       <c r="W29" s="7"/>
       <c r="X29" s="12"/>
     </row>
-    <row r="30" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="65">
         <v>29</v>
       </c>
@@ -8663,7 +8677,7 @@
       </c>
       <c r="X30" s="9"/>
     </row>
-    <row r="31" spans="1:24" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="65">
         <v>30</v>
       </c>
@@ -8735,7 +8749,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="32" spans="1:24" s="2" customFormat="1" ht="195" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" s="2" customFormat="1" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="65">
         <v>31</v>
       </c>
@@ -8876,7 +8890,7 @@
       </c>
       <c r="Y33" s="15"/>
     </row>
-    <row r="34" spans="1:25" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="65">
         <v>33</v>
       </c>
@@ -9368,7 +9382,7 @@
       </c>
       <c r="X40" s="7"/>
     </row>
-    <row r="41" spans="1:25" s="2" customFormat="1" ht="165" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" s="2" customFormat="1" ht="165" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="65">
         <v>40</v>
       </c>
@@ -9436,7 +9450,7 @@
       <c r="W41" s="20"/>
       <c r="X41" s="7"/>
     </row>
-    <row r="42" spans="1:25" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" s="2" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="65">
         <v>41</v>
       </c>
@@ -9506,7 +9520,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="43" spans="1:25" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="65">
         <v>42</v>
       </c>
@@ -9576,7 +9590,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="44" spans="1:25" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="65">
         <v>43</v>
       </c>
@@ -9646,7 +9660,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="45" spans="1:25" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" s="2" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="65">
         <v>44</v>
       </c>
@@ -9718,7 +9732,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="46" spans="1:25" s="2" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" s="2" customFormat="1" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="65">
         <v>45</v>
       </c>
@@ -9786,7 +9800,7 @@
       </c>
       <c r="X46" s="75"/>
     </row>
-    <row r="47" spans="1:25" s="2" customFormat="1" ht="142.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" s="2" customFormat="1" ht="142.5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="65">
         <v>46</v>
       </c>
@@ -9856,7 +9870,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="48" spans="1:25" s="2" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" s="2" customFormat="1" ht="135" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="65">
         <v>47</v>
       </c>
@@ -9926,7 +9940,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="49" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="65">
         <v>48</v>
       </c>
@@ -9992,7 +10006,7 @@
       </c>
       <c r="X49" s="7"/>
     </row>
-    <row r="50" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="65">
         <v>49</v>
       </c>
@@ -10058,7 +10072,7 @@
       </c>
       <c r="X50" s="78"/>
     </row>
-    <row r="51" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="65">
         <v>50</v>
       </c>
@@ -10124,7 +10138,7 @@
       </c>
       <c r="X51" s="12"/>
     </row>
-    <row r="52" spans="1:24" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" s="2" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="65">
         <v>51</v>
       </c>
@@ -10192,7 +10206,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="53" spans="1:24" s="2" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" s="2" customFormat="1" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="65">
         <v>52</v>
       </c>
@@ -10260,7 +10274,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="54" spans="1:24" s="2" customFormat="1" ht="150" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" s="2" customFormat="1" ht="150" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="65">
         <v>53</v>
       </c>
@@ -10332,7 +10346,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="55" spans="1:24" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="65">
         <v>54</v>
       </c>
@@ -10404,7 +10418,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="56" spans="1:24" s="2" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" s="2" customFormat="1" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="65">
         <v>55</v>
       </c>
@@ -10476,7 +10490,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="57" spans="1:24" s="2" customFormat="1" ht="180" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" s="2" customFormat="1" ht="180" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="65">
         <v>56</v>
       </c>
@@ -10548,7 +10562,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="58" spans="1:24" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" s="2" customFormat="1" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="65">
         <v>57</v>
       </c>
@@ -10618,7 +10632,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="59" spans="1:24" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" s="2" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="65">
         <v>58</v>
       </c>
@@ -10894,7 +10908,7 @@
       <c r="W62" s="9"/>
       <c r="X62" s="7"/>
     </row>
-    <row r="63" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="65">
         <v>62</v>
       </c>
@@ -10964,7 +10978,7 @@
       </c>
       <c r="X63" s="7"/>
     </row>
-    <row r="64" spans="1:24" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" s="2" customFormat="1" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="65">
         <v>63</v>
       </c>
@@ -11796,7 +11810,7 @@
       <c r="Z75" s="77"/>
       <c r="AB75" s="77"/>
     </row>
-    <row r="76" spans="1:28" ht="75" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:28" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="70">
         <v>75</v>
       </c>
@@ -11867,7 +11881,7 @@
       <c r="Z76" s="77"/>
       <c r="AB76" s="77"/>
     </row>
-    <row r="77" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="70">
         <v>76</v>
       </c>
@@ -11936,7 +11950,7 @@
       <c r="Z77" s="77"/>
       <c r="AB77" s="77"/>
     </row>
-    <row r="78" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="70">
         <v>77</v>
       </c>
@@ -12074,7 +12088,7 @@
       <c r="Z79" s="77"/>
       <c r="AB79" s="77"/>
     </row>
-    <row r="80" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="70">
         <v>79</v>
       </c>
@@ -12141,7 +12155,7 @@
       <c r="Z80" s="77"/>
       <c r="AB80" s="77"/>
     </row>
-    <row r="81" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="70">
         <v>80</v>
       </c>
@@ -12210,7 +12224,7 @@
       <c r="Z81" s="77"/>
       <c r="AB81" s="77"/>
     </row>
-    <row r="82" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="65">
         <v>81</v>
       </c>
@@ -12279,7 +12293,7 @@
       <c r="Z82" s="77"/>
       <c r="AB82" s="77"/>
     </row>
-    <row r="83" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:28" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="70">
         <v>82</v>
       </c>
@@ -12348,7 +12362,7 @@
       <c r="Z83" s="77"/>
       <c r="AB83" s="77"/>
     </row>
-    <row r="84" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:28" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="70">
         <v>83</v>
       </c>
@@ -12417,7 +12431,7 @@
       <c r="Z84" s="77"/>
       <c r="AB84" s="77"/>
     </row>
-    <row r="85" spans="1:28" ht="75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:28" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="70">
         <v>84</v>
       </c>
@@ -12464,7 +12478,7 @@
       <c r="Z85" s="77"/>
       <c r="AB85" s="77"/>
     </row>
-    <row r="86" spans="1:28" ht="75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:28" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="65">
         <v>85</v>
       </c>
@@ -12509,7 +12523,7 @@
       <c r="Z86" s="77"/>
       <c r="AB86" s="77"/>
     </row>
-    <row r="87" spans="1:28" ht="75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:28" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="70">
         <v>86</v>
       </c>
@@ -14070,12 +14084,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004309D8389C5A084A8EB9FED342634609" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c1ee2663b349001e41875756695405cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e8508775-6f2a-451e-b0c0-0da0ba3b654b" xmlns:ns3="f15e5eab-f649-4efd-a2c2-4935b72130ea" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d6561bc30f91fc8f80cc55469271a584" ns2:_="" ns3:_="">
     <xsd:import namespace="e8508775-6f2a-451e-b0c0-0da0ba3b654b"/>
@@ -14240,6 +14248,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -14250,15 +14264,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6ECE83-F240-478D-BE60-3B98A1630AA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EA6218BD-C386-4EBA-AE3F-6A1B03CAFB13}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -14277,6 +14282,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE6ECE83-F240-478D-BE60-3B98A1630AA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{91500E67-CFBD-4E57-93CA-25297AD67667}">
   <ds:schemaRefs>

</xml_diff>